<commit_message>
Testcase atualizado com resultado
</commit_message>
<xml_diff>
--- a/Casos de testes - Sauce  Demo.xlsx
+++ b/Casos de testes - Sauce  Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PastaTreinamento\aulaTestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAE89A78-FF5C-439D-BE67-E92ED5A8AC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB37D888-37AE-4C62-B7A0-57D838ED4212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="137">
   <si>
     <t>ID</t>
   </si>
@@ -145,12 +145,6 @@
     <t>Iniciar checkout</t>
   </si>
   <si>
-    <t>Preencher dados obrigatórios</t>
-  </si>
-  <si>
-    <t>Campos obrigatórios em branco</t>
-  </si>
-  <si>
     <t>Finalizar compra com sucesso</t>
   </si>
   <si>
@@ -277,9 +271,6 @@
     <t>Clicar em 'Checkout'</t>
   </si>
   <si>
-    <t>Nome, sobrenome, CEP</t>
-  </si>
-  <si>
     <t>Campos vazios</t>
   </si>
   <si>
@@ -298,9 +289,6 @@
     <t>Reduzir/alterar o tamanho da janela</t>
   </si>
   <si>
-    <t>Usar Tab, Alt, Aria tags</t>
-  </si>
-  <si>
     <t>Redirecionar para a página de produtos</t>
   </si>
   <si>
@@ -316,9 +304,6 @@
     <t>Login permitido, verificar anomalias na UI</t>
   </si>
   <si>
-    <t>Exibir 6 itens com nome, descrição e preço</t>
-  </si>
-  <si>
     <t>Produtos listados de A a Z</t>
   </si>
   <si>
@@ -374,13 +359,97 @@
   </si>
   <si>
     <t>Passou</t>
+  </si>
+  <si>
+    <t>Exibir 6 itens com nome, descrição e preço ($0,00)</t>
+  </si>
+  <si>
+    <t>BLOQUEADO</t>
+  </si>
+  <si>
+    <t>Obs: Descricao do teste nao esta clara</t>
+  </si>
+  <si>
+    <t>Nome, sobrenome, Codigo postal</t>
+  </si>
+  <si>
+    <t>Your Information - Preencher dados obrigatórios</t>
+  </si>
+  <si>
+    <t>Your Information - Campos obrigatórios em branco</t>
+  </si>
+  <si>
+    <t>Obs: Validar se fluxo esta ideal (Feature)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Usar Tab, Alt, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aria tags</t>
+    </r>
+  </si>
+  <si>
+    <t>Obs: Dificil visualização do campo/botao selecionado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Bloqueados</t>
+  </si>
+  <si>
+    <t>Obs: Valor for a do padrao ($0.00)</t>
+  </si>
+  <si>
+    <t>1#BUG</t>
+  </si>
+  <si>
+    <t>Formato do valor esta incorreto</t>
+  </si>
+  <si>
+    <t>Ao acessar a pagina de produto, destacamos que o valor esta fora do padrao solicitado</t>
+  </si>
+  <si>
+    <t>Evidencia:</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>Severidade</t>
+  </si>
+  <si>
+    <t>Titulo</t>
+  </si>
+  <si>
+    <t>Anexos</t>
+  </si>
+  <si>
+    <t>2#BUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navegaçao por TAB </t>
+  </si>
+  <si>
+    <t>Nao ha retorno visual para o campo/botao em destaque</t>
+  </si>
+  <si>
+    <t>Baixa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,8 +479,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +509,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -453,22 +541,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,6 +573,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>385050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>137948</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>119568</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>189656</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D584C71-7595-C401-56CB-20289D3C1E7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17103067" y="2042948"/>
+          <a:ext cx="4621828" cy="2147208"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>13138</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38878</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>460939</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>129016</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3895BDA7-ABD3-C263-7B37-F7BD8C501FE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16731155" y="229378"/>
+          <a:ext cx="2891456" cy="1423638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>683173</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>52551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3574629</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>142689</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCE68DB1-12BA-4A47-88D2-FFBE97B3B313}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10346121" y="5958051"/>
+          <a:ext cx="2891456" cy="1423638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>111673</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>25724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>364777</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>158334</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1B9E6ED-B44A-37A6-F4DC-E3C6C5670DF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9774621" y="7645724"/>
+          <a:ext cx="4003984" cy="1656610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -771,22 +1043,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,10 +1077,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -814,19 +1088,19 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -834,19 +1108,19 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -854,16 +1128,19 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -871,16 +1148,19 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -888,16 +1168,19 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -905,16 +1188,22 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -922,16 +1211,19 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -939,16 +1231,19 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -956,16 +1251,22 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -973,16 +1274,19 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -990,16 +1294,19 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1007,16 +1314,19 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1024,16 +1334,19 @@
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1041,152 +1354,267 @@
         <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>114</v>
+      </c>
+      <c r="G23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>